<commit_message>
Calendar + Addressbook - new template files
Change-Id: Ib155aeed48517f2eb7cfd052995e73cc2151377d
Reviewed-on: http://gerrit.tine20.com/customers/5475
Tested-by: Jenkins CI (http://ci.tine20.com/) <tine20-jenkins@metaways.de>
Reviewed-by: Paul Mehrer <p.mehrer@metaways.de>
Tested-by: Paul Mehrer <p.mehrer@metaways.de>
</commit_message>
<xml_diff>
--- a/tine20/Addressbook/Export/templates/addressbook_contact_overview.xlsx
+++ b/tine20/Addressbook/Export/templates/addressbook_contact_overview.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzornsch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzornsch/Desktop/Lokal_2017-08-01/Standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -59,9 +59,6 @@
     <t>${twig:translate('Title')}</t>
   </si>
   <si>
-    <t>${twig:record.title}</t>
-  </si>
-  <si>
     <t>${twig:translate('First Name')}</t>
   </si>
   <si>
@@ -96,38 +93,19 @@
   </si>
   <si>
     <t>${twig:record.email}${/ROW}</t>
+  </si>
+  <si>
+    <t>${twig:record.n_prefix}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri (Textkörper)"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF4472C4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -153,6 +131,38 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF4472C4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -195,30 +205,38 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -343,7 +361,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6745125" y="47037"/>
+          <a:off x="8456803" y="47037"/>
           <a:ext cx="1972405" cy="481584"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -619,139 +637,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="110" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="30.33203125" customWidth="1"/>
-    <col min="9" max="9" width="28.5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="11.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17" style="7" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="7" customWidth="1"/>
+    <col min="8" max="8" width="37.5" style="7" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="7" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="7" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
     </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="E6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="9" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.51" footer="0.51"/>
-  <pageSetup paperSize="9" scale="88" firstPageNumber="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <colBreaks count="1" manualBreakCount="1">
-    <brk id="10" max="1048575" man="1"/>
-  </colBreaks>
+  <pageSetup paperSize="9" scale="83" firstPageNumber="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feature(Addressbook/Export): add address infos to xls
... overview template
</commit_message>
<xml_diff>
--- a/tine20/Addressbook/Export/templates/addressbook_contact_overview.xlsx
+++ b/tine20/Addressbook/Export/templates/addressbook_contact_overview.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelius/src/tine20.git/tine20/Addressbook/Export/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzornsch/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149878BD-4C50-F645-8D52-C8D10EBC93FC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58431A8-DA91-DE4A-9DF0-EA6CCEB5FB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1700" yWindow="4180" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>${twig:branding.title}</t>
   </si>
@@ -85,13 +94,31 @@
   </si>
   <si>
     <t>${ROW}${twig:keyField('Addressbook','contactSalutation',record.salutation)}</t>
+  </si>
+  <si>
+    <t>${twig:translate('Street')}</t>
+  </si>
+  <si>
+    <t>${twig:record.adr_one_street}</t>
+  </si>
+  <si>
+    <t>${twig:record.adr_one_postalcode}</t>
+  </si>
+  <si>
+    <t>${twig:record.adr_one_locality}</t>
+  </si>
+  <si>
+    <t>${twig:translate('Postal Code')}</t>
+  </si>
+  <si>
+    <t>${twig:translate('City')}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -152,6 +179,12 @@
       <color rgb="FF4472C4"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -199,7 +232,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -228,12 +261,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -321,13 +355,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>112903</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>2085308</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>528621</xdr:rowOff>
@@ -635,23 +669,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="11.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="17" style="7" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="7" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="7"/>
+    <col min="5" max="6" width="22.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="7" customWidth="1"/>
+    <col min="11" max="11" width="33.33203125" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -661,8 +699,11 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -672,9 +713,12 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -684,9 +728,12 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
     </row>
-    <row r="5" spans="1:8" s="11" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" s="11" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
@@ -703,16 +750,25 @@
         <v>8</v>
       </c>
       <c r="F5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="8" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -729,19 +785,28 @@
         <v>12</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="K6" s="9" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.51" footer="0.51"/>
-  <pageSetup paperSize="9" scale="86" firstPageNumber="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" scale="61" firstPageNumber="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>